<commit_message>
Ajuste nas classes, Adicionando Page Object
</commit_message>
<xml_diff>
--- a/BolsaValores.xlsx
+++ b/BolsaValores.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Auditeste0151\Desktop\"/>
     </mc:Choice>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="74">
   <si>
     <t xml:space="preserve">Código </t>
   </si>
@@ -58,12 +58,208 @@
   </si>
   <si>
     <t>JPY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    BRL</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>0,1960</t>
+  </si>
+  <si>
+    <t>0,1761</t>
+  </si>
+  <si>
+    <t>0,1574</t>
+  </si>
+  <si>
+    <t>21,1615</t>
+  </si>
+  <si>
+    <t>0,1866</t>
+  </si>
+  <si>
+    <t>0,2741</t>
+  </si>
+  <si>
+    <t>0,3180</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    USD</t>
+  </si>
+  <si>
+    <t>5,1010</t>
+  </si>
+  <si>
+    <t>0,8974</t>
+  </si>
+  <si>
+    <t>0,8040</t>
+  </si>
+  <si>
+    <t>107,94</t>
+  </si>
+  <si>
+    <t>0,9513</t>
+  </si>
+  <si>
+    <t>1,3979</t>
+  </si>
+  <si>
+    <t>1,6221</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    EUR</t>
+  </si>
+  <si>
+    <t>5,6836</t>
+  </si>
+  <si>
+    <t>1,1143</t>
+  </si>
+  <si>
+    <t>0,8958</t>
+  </si>
+  <si>
+    <t>120,27</t>
+  </si>
+  <si>
+    <t>1,0604</t>
+  </si>
+  <si>
+    <t>1,5581</t>
+  </si>
+  <si>
+    <t>1,8082</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    GBP</t>
+  </si>
+  <si>
+    <t>6,3548</t>
+  </si>
+  <si>
+    <t>1,2439</t>
+  </si>
+  <si>
+    <t>1,1180</t>
+  </si>
+  <si>
+    <t>134,26</t>
+  </si>
+  <si>
+    <t>1,1834</t>
+  </si>
+  <si>
+    <t>1,7394</t>
+  </si>
+  <si>
+    <t>2,0177</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    JPY</t>
+  </si>
+  <si>
+    <t>0,04725</t>
+  </si>
+  <si>
+    <t>0,00926</t>
+  </si>
+  <si>
+    <t>0,00832</t>
+  </si>
+  <si>
+    <t>0,00744</t>
+  </si>
+  <si>
+    <t>0,0088</t>
+  </si>
+  <si>
+    <t>0,01295</t>
+  </si>
+  <si>
+    <t>0,01504</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    CHF</t>
+  </si>
+  <si>
+    <t>5,3602</t>
+  </si>
+  <si>
+    <t>1,0512</t>
+  </si>
+  <si>
+    <t>0,9431</t>
+  </si>
+  <si>
+    <t>0,8449</t>
+  </si>
+  <si>
+    <t>113,47</t>
+  </si>
+  <si>
+    <t>1,4700</t>
+  </si>
+  <si>
+    <t>1,7051</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    CAD</t>
+  </si>
+  <si>
+    <t>3,6479</t>
+  </si>
+  <si>
+    <t>0,7154</t>
+  </si>
+  <si>
+    <t>0,6420</t>
+  </si>
+  <si>
+    <t>0,5743</t>
+  </si>
+  <si>
+    <t>77,19</t>
+  </si>
+  <si>
+    <t>0,6806</t>
+  </si>
+  <si>
+    <t>1,1602</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    AUD</t>
+  </si>
+  <si>
+    <t>3,1449</t>
+  </si>
+  <si>
+    <t>0,6165</t>
+  </si>
+  <si>
+    <t>0,5534</t>
+  </si>
+  <si>
+    <t>0,4955</t>
+  </si>
+  <si>
+    <t>66,55</t>
+  </si>
+  <si>
+    <t>0,5865</t>
+  </si>
+  <si>
+    <t>0,8620</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -458,7 +654,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95E2D11F-7474-4867-9558-C82B188A2BE0}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
@@ -466,8 +662,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" customWidth="1"/>
-    <col min="2" max="9" width="10.28515625" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="2" max="9" customWidth="true" width="10.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -499,16 +695,237 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" t="s">
+        <v>39</v>
+      </c>
+      <c r="H5" t="s">
+        <v>40</v>
+      </c>
+      <c r="I5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" t="s">
+        <v>47</v>
+      </c>
+      <c r="H6" t="s">
+        <v>48</v>
+      </c>
+      <c r="I6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D7" t="s">
+        <v>53</v>
+      </c>
+      <c r="E7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F7" t="s">
+        <v>55</v>
+      </c>
+      <c r="G7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" t="s">
+        <v>56</v>
+      </c>
+      <c r="I7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D8" t="s">
+        <v>61</v>
+      </c>
+      <c r="E8" t="s">
+        <v>62</v>
+      </c>
+      <c r="F8" t="s">
+        <v>63</v>
+      </c>
+      <c r="G8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H8" t="s">
+        <v>10</v>
+      </c>
+      <c r="I8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D9" t="s">
+        <v>69</v>
+      </c>
+      <c r="E9" t="s">
+        <v>70</v>
+      </c>
+      <c r="F9" t="s">
+        <v>71</v>
+      </c>
+      <c r="G9" t="s">
+        <v>72</v>
+      </c>
+      <c r="H9" t="s">
+        <v>73</v>
+      </c>
+      <c r="I9" t="s">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>